<commit_message>
Filtros ainda nao funcionando
</commit_message>
<xml_diff>
--- a/src/DE-PARA_FUNCOES.xlsx
+++ b/src/DE-PARA_FUNCOES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mar21\Documents\Trabalho\CGINF\Projetos_R\Etnia_genero\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{717DDABD-C69C-453D-971C-5367FF990C96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB505E3-D016-4264-BAE8-20F3168D97A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="-4245" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1351,7 +1351,7 @@
   <dimension ref="A1:D276"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>